<commit_message>
Matriz de trabajo - Historias de usuario V1.4
</commit_message>
<xml_diff>
--- a/PREGAME/1. ELICITACION/1.3 Historias de usuario/G1_Matriz de Marco de Trabajo HU_V1.4.xlsx
+++ b/PREGAME/1. ELICITACION/1.3 Historias de usuario/G1_Matriz de Marco de Trabajo HU_V1.4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reishel\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5790545A-0B2E-4074-86AF-6845ECBDA7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D478F7A2-8B32-4408-AF48-1A1A3A4B37DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato descripción HU" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="177">
   <si>
     <t>Matriz de Marco de Trabajo de HU</t>
   </si>
@@ -469,9 +469,6 @@
     <t>Acceder a "Modificar contraseña", ingresar contraseña actual, nueva y confirmación, y guardar cambios.</t>
   </si>
   <si>
-    <t>(Asignar)</t>
-  </si>
-  <si>
     <t>Se valida contraseña actual; nueva cumple políticas; confirmación coincide; mensaje “Contraseña actualizada correctamente”.</t>
   </si>
   <si>
@@ -592,6 +589,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -599,10 +597,12 @@
       <sz val="16"/>
       <color theme="1"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -610,50 +610,59 @@
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="16"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -661,17 +670,20 @@
       <sz val="12"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1515,8 +1527,8 @@
   </sheetPr>
   <dimension ref="A1:AF999"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E6" zoomScale="66" zoomScaleNormal="66" workbookViewId="0">
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.69921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1708,25 +1720,25 @@
         <v>15</v>
       </c>
       <c r="C6" s="38" t="s">
+        <v>144</v>
+      </c>
+      <c r="D6" s="38" t="s">
         <v>145</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="E6" s="38" t="s">
         <v>146</v>
-      </c>
-      <c r="E6" s="38" t="s">
-        <v>147</v>
       </c>
       <c r="F6" s="36" t="s">
         <v>140</v>
       </c>
       <c r="G6" s="38" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H6" s="38" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="38">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J6" s="39">
         <v>45996</v>
@@ -1738,13 +1750,13 @@
         <v>23</v>
       </c>
       <c r="M6" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6" s="38" t="s">
         <v>149</v>
       </c>
-      <c r="N6" s="38" t="s">
+      <c r="O6" s="38" t="s">
         <v>150</v>
-      </c>
-      <c r="O6" s="38" t="s">
-        <v>151</v>
       </c>
       <c r="P6" s="28"/>
       <c r="Q6" s="1"/>
@@ -1794,13 +1806,13 @@
         <v>23</v>
       </c>
       <c r="M7" s="42" t="s">
+        <v>142</v>
+      </c>
+      <c r="N7" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="N7" s="42" t="s">
-        <v>144</v>
-      </c>
       <c r="O7" s="42" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="P7" s="28"/>
       <c r="Q7" s="1"/>
@@ -1843,7 +1855,7 @@
         <v>53</v>
       </c>
       <c r="I8" s="36">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J8" s="37">
         <v>45979</v>
@@ -1861,7 +1873,7 @@
         <v>25</v>
       </c>
       <c r="O8" s="36" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="P8" s="28"/>
       <c r="Q8" s="1"/>
@@ -1904,7 +1916,7 @@
         <v>100</v>
       </c>
       <c r="I9" s="30">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J9" s="31">
         <v>45979</v>
@@ -1922,7 +1934,7 @@
         <v>32</v>
       </c>
       <c r="O9" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="1"/>
@@ -1985,7 +1997,7 @@
         <v>39</v>
       </c>
       <c r="O10" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="1"/>
@@ -2046,7 +2058,7 @@
         <v>47</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="P11" s="28"/>
       <c r="Q11" s="1"/>
@@ -2066,19 +2078,19 @@
         <v>64</v>
       </c>
       <c r="C12" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D12" s="38" t="s">
         <v>155</v>
       </c>
-      <c r="D12" s="38" t="s">
+      <c r="E12" s="38" t="s">
         <v>156</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>157</v>
       </c>
       <c r="F12" s="38" t="s">
         <v>19</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H12" s="38" t="s">
         <v>53</v>
@@ -2096,13 +2108,13 @@
         <v>23</v>
       </c>
       <c r="M12" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="N12" s="38" t="s">
         <v>159</v>
       </c>
-      <c r="N12" s="38" t="s">
-        <v>160</v>
-      </c>
       <c r="O12" s="38" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="P12" s="28"/>
       <c r="Q12" s="1"/>
@@ -2140,7 +2152,7 @@
         <v>53</v>
       </c>
       <c r="I13" s="36">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J13" s="37">
         <v>45979</v>
@@ -2158,7 +2170,7 @@
         <v>55</v>
       </c>
       <c r="O13" s="36" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="P13" s="28"/>
       <c r="Q13" s="1"/>
@@ -2214,7 +2226,7 @@
         <v>111</v>
       </c>
       <c r="O14" s="30" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="P14" s="28"/>
       <c r="Q14" s="1"/>
@@ -2252,7 +2264,7 @@
         <v>53</v>
       </c>
       <c r="I15" s="30">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="J15" s="31">
         <v>45979</v>
@@ -2326,7 +2338,7 @@
         <v>70</v>
       </c>
       <c r="O16" s="30" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="P16" s="28"/>
       <c r="Q16" s="1"/>
@@ -2364,7 +2376,7 @@
         <v>76</v>
       </c>
       <c r="I17" s="30">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J17" s="31">
         <v>45979</v>
@@ -2382,7 +2394,7 @@
         <v>78</v>
       </c>
       <c r="O17" s="30" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="P17" s="28"/>
       <c r="Q17" s="1"/>
@@ -2476,7 +2488,7 @@
         <v>76</v>
       </c>
       <c r="I19" s="46">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J19" s="47">
         <v>45979</v>
@@ -2520,22 +2532,22 @@
         <v>136</v>
       </c>
       <c r="C20" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="38" t="s">
         <v>171</v>
       </c>
-      <c r="D20" s="38" t="s">
+      <c r="E20" s="38" t="s">
         <v>172</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>173</v>
       </c>
       <c r="F20" s="38" t="s">
         <v>19</v>
       </c>
       <c r="G20" s="38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H20" s="38" t="s">
-        <v>142</v>
+        <v>21</v>
       </c>
       <c r="I20" s="38">
         <v>5</v>
@@ -2550,13 +2562,13 @@
         <v>23</v>
       </c>
       <c r="M20" s="38" t="s">
+        <v>174</v>
+      </c>
+      <c r="N20" s="38" t="s">
         <v>175</v>
       </c>
-      <c r="N20" s="38" t="s">
-        <v>176</v>
-      </c>
       <c r="O20" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="P20" s="28"/>
       <c r="Q20" s="1"/>
@@ -2579,7 +2591,7 @@
     <row r="21" spans="1:32" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="28"/>
       <c r="B21" s="45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C21" s="36" t="s">
         <v>113</v>
@@ -2591,7 +2603,7 @@
         <v>115</v>
       </c>
       <c r="F21" s="36" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G21" s="36" t="s">
         <v>116</v>
@@ -2600,7 +2612,7 @@
         <v>100</v>
       </c>
       <c r="I21" s="36">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J21" s="37">
         <v>45979</v>
@@ -2635,7 +2647,7 @@
     <row r="22" spans="1:32" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="28"/>
       <c r="B22" s="44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C22" s="48" t="s">
         <v>96</v>
@@ -2656,7 +2668,7 @@
         <v>100</v>
       </c>
       <c r="I22" s="30">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="J22" s="31">
         <v>45979</v>
@@ -30229,7 +30241,7 @@
       <c r="B13" s="26"/>
       <c r="C13" s="12">
         <f>VLOOKUP('Historia de Usuario'!C10,'Formato descripción HU'!B6:O23,8,0)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D13" s="13"/>
       <c r="E13" s="69" t="str">

</xml_diff>